<commit_message>
modefy data_standardization script to translte data from Dutch to English and update new genearted excel sheets for T0,1,2 and 3 in cleaned fol
</commit_message>
<xml_diff>
--- a/data/cleaned/cw_T0_cleaned.xlsx
+++ b/data/cleaned/cw_T0_cleaned.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Monsteromschrijving</t>
+          <t>Sample description</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -456,67 +456,67 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Ijzer (2+)</t>
+          <t>Iron II</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Mangaan (II)</t>
+          <t>MN II</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>cyanide (totaal)</t>
+          <t>cyanid</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>fosfor (totaal)</t>
+          <t>phosphor</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>benzeen</t>
+          <t>benzene</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>tolueen</t>
+          <t>toluene</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>ethylbenzeen</t>
+          <t>ethylbenzene</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>o-xyleen</t>
+          <t>o-xylene</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>p- en m-xyleen</t>
+          <t>(m+p)-xylene</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>xylenen (0.7 factor)</t>
+          <t>sum xylenes (factor 0.7)</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>totaal BTEX (0.7 factor)</t>
+          <t>total BTEX (factor 0.7)</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>naftaleen</t>
+          <t>naphthalene</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>fenol</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
@@ -536,67 +536,67 @@
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>som cresolen</t>
+          <t>som cresols</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>2-ethylfenol</t>
+          <t>2-ethylphenol</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>3-ethylfenol</t>
+          <t>3-ethylphenol</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>2,4-dimethylfenol</t>
+          <t>2,4-dimethylphenol</t>
         </is>
       </c>
       <c r="Y1" t="inlineStr">
         <is>
-          <t>2,5-dimethylfenol</t>
+          <t>2,5-dimethylphenol</t>
         </is>
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>3,5+2,3-dimethylfenol+4-ethylfenol</t>
+          <t>3,5+2,3-dimethylphenol+4-ethylphenol</t>
         </is>
       </c>
       <c r="AA1" t="inlineStr">
         <is>
-          <t>2,6-dimethylfenol</t>
+          <t>2,6-dimethylphenol</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>3,4-dimethylfenol</t>
+          <t>3,4-dimethylphenol</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>som C2-alkylfenolen</t>
+          <t>som C2-alkylphenolen</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>2,3,5-trimethylfenol</t>
+          <t>2,3,5-trimethylphenol</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>3,4,5-trimethylfenol</t>
+          <t>3,4,5-trimethylphenol</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>2-isopropylfenol</t>
+          <t>2-isopropylphenol</t>
         </is>
       </c>
       <c r="AG1" t="inlineStr">
         <is>
-          <t>som C3-alkylfenolen</t>
+          <t>som C3-alkylphenolen</t>
         </is>
       </c>
       <c r="AH1" t="inlineStr">
@@ -606,52 +606,52 @@
       </c>
       <c r="AI1" t="inlineStr">
         <is>
-          <t>p-(tert)butylfenol</t>
+          <t>p-(tert)butylphenol</t>
         </is>
       </c>
       <c r="AJ1" t="inlineStr">
         <is>
-          <t>som C4-alkylfenolen</t>
+          <t>som C4-alkylphenolen</t>
         </is>
       </c>
       <c r="AK1" t="inlineStr">
         <is>
-          <t>naftaleen</t>
+          <t>naphthalene</t>
         </is>
       </c>
       <c r="AL1" t="inlineStr">
         <is>
-          <t>acenaftyleen</t>
+          <t>acenaphthylene</t>
         </is>
       </c>
       <c r="AM1" t="inlineStr">
         <is>
-          <t>acenafteen</t>
+          <t>acenaphtene</t>
         </is>
       </c>
       <c r="AN1" t="inlineStr">
         <is>
-          <t>fluoreen</t>
+          <t>fluorene</t>
         </is>
       </c>
       <c r="AO1" t="inlineStr">
         <is>
-          <t>fenantreen</t>
+          <t>phenanthrene</t>
         </is>
       </c>
       <c r="AP1" t="inlineStr">
         <is>
-          <t>antraceen</t>
+          <t>anthracene</t>
         </is>
       </c>
       <c r="AQ1" t="inlineStr">
         <is>
-          <t>fluoranteen</t>
+          <t>fluoranthene</t>
         </is>
       </c>
       <c r="AR1" t="inlineStr">
         <is>
-          <t>pyreen</t>
+          <t>pyrene</t>
         </is>
       </c>
       <c r="AS1" t="inlineStr">
@@ -661,72 +661,72 @@
       </c>
       <c r="AT1" t="inlineStr">
         <is>
-          <t>chryseen</t>
+          <t>chrysene</t>
         </is>
       </c>
       <c r="AU1" t="inlineStr">
         <is>
-          <t>benzo(b)fluoranteen</t>
+          <t>benzo(b)fluoranthene</t>
         </is>
       </c>
       <c r="AV1" t="inlineStr">
         <is>
-          <t>benzo(k)fluoranteen</t>
+          <t>benzo(k)fluoranthene</t>
         </is>
       </c>
       <c r="AW1" t="inlineStr">
         <is>
-          <t>benzo(a)pyreen</t>
+          <t>benzo(a)pyrene</t>
         </is>
       </c>
       <c r="AX1" t="inlineStr">
         <is>
-          <t>dibenz(a,h)antraceen</t>
+          <t>dibenz(a,h)anthracene</t>
         </is>
       </c>
       <c r="AY1" t="inlineStr">
         <is>
-          <t>benzo(ghi)peryleen</t>
+          <t>benzo(g,h,i)perylene</t>
         </is>
       </c>
       <c r="AZ1" t="inlineStr">
         <is>
-          <t>indeno(1,2,3-cd)pyreen</t>
+          <t>indeno(1,2,3-cd)pyrene</t>
         </is>
       </c>
       <c r="BA1" t="inlineStr">
         <is>
-          <t>pak-totaal (16 van EPA)</t>
+          <t>sum PAH (16 EPA)</t>
         </is>
       </c>
       <c r="BB1" t="inlineStr">
         <is>
-          <t>pak-totaal (10 van VROM) (0.7 factor)</t>
+          <t>sum PAH (VROM) (factor 0.7)</t>
         </is>
       </c>
       <c r="BC1" t="inlineStr">
         <is>
-          <t>fractie C10-C12</t>
+          <t>fraction C10-C12</t>
         </is>
       </c>
       <c r="BD1" t="inlineStr">
         <is>
-          <t>fractie C12-C22</t>
+          <t>fraction C12-C22</t>
         </is>
       </c>
       <c r="BE1" t="inlineStr">
         <is>
-          <t>fractie C22-C30</t>
+          <t>fraction C22-C30</t>
         </is>
       </c>
       <c r="BF1" t="inlineStr">
         <is>
-          <t>fractie C30-C40</t>
+          <t>fraction C30-C40</t>
         </is>
       </c>
       <c r="BG1" t="inlineStr">
         <is>
-          <t>totaal olie C10 - C40</t>
+          <t>total oil C10 - C40</t>
         </is>
       </c>
       <c r="BH1" t="inlineStr">
@@ -736,32 +736,32 @@
       </c>
       <c r="BI1" t="inlineStr">
         <is>
-          <t>nitriet</t>
+          <t>nitrite</t>
         </is>
       </c>
       <c r="BJ1" t="inlineStr">
         <is>
-          <t>nitriet</t>
+          <t>nitrite - N</t>
         </is>
       </c>
       <c r="BK1" t="inlineStr">
         <is>
-          <t>nitraat</t>
+          <t>nitrate</t>
         </is>
       </c>
       <c r="BL1" t="inlineStr">
         <is>
-          <t>nitraat</t>
+          <t>nitrate - N</t>
         </is>
       </c>
       <c r="BM1" t="inlineStr">
         <is>
-          <t>sulfaat</t>
+          <t>sulphates</t>
         </is>
       </c>
       <c r="BN1" t="inlineStr">
         <is>
-          <t>Zuurstof</t>
+          <t>Oxygen</t>
         </is>
       </c>
     </row>

</xml_diff>